<commit_message>
Added the sli.do questions/comments
</commit_message>
<xml_diff>
--- a/2019/slido/Questions-SCAM 2019.xlsx
+++ b/2019/slido/Questions-SCAM 2019.xlsx
@@ -3,9 +3,9 @@
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="5" rupBuild="21425"/>
   <workbookPr filterPrivacy="1"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{FFDAEF55-D613-42D0-A85D-AF98BD16C598}" xr6:coauthVersionLast="43" xr6:coauthVersionMax="43" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1DE04CF5-8BD4-4C8D-A2D3-5579D748432B}" xr6:coauthVersionLast="43" xr6:coauthVersionMax="43" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" firstSheet="1" activeTab="4" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Program Analysis" sheetId="2" r:id="rId1"/>
@@ -776,8 +776,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
   <dimension ref="A1:I20"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A10" workbookViewId="0">
-      <selection activeCell="A19" sqref="A19"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="G16" sqref="G16"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="15"/>
@@ -785,9 +785,9 @@
     <col min="1" max="1" width="91.85546875" customWidth="1"/>
     <col min="2" max="2" width="6.42578125" customWidth="1"/>
     <col min="3" max="3" width="8.85546875" customWidth="1"/>
-    <col min="4" max="4" width="13.42578125" customWidth="1"/>
+    <col min="4" max="4" width="6" customWidth="1"/>
     <col min="5" max="5" width="2.5703125" customWidth="1"/>
-    <col min="6" max="6" width="15.5703125" customWidth="1"/>
+    <col min="6" max="6" width="13.42578125" customWidth="1"/>
     <col min="7" max="7" width="27.140625" customWidth="1"/>
     <col min="8" max="9" width="18" customWidth="1"/>
   </cols>
@@ -1383,11 +1383,13 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0200-000000000000}">
   <dimension ref="A1:I14"/>
   <sheetViews>
-    <sheetView workbookViewId="0"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A8" sqref="A8"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="15"/>
   <cols>
-    <col min="1" max="1" width="35.28515625" customWidth="1"/>
+    <col min="1" max="1" width="93.85546875" customWidth="1"/>
     <col min="2" max="2" width="6.42578125" customWidth="1"/>
     <col min="3" max="3" width="8.85546875" customWidth="1"/>
     <col min="4" max="4" width="13.42578125" customWidth="1"/>
@@ -1814,7 +1816,9 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0300-000000000000}">
   <dimension ref="A1:I7"/>
   <sheetViews>
-    <sheetView workbookViewId="0"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A7" sqref="A7"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="15"/>
   <cols>
@@ -2098,8 +2102,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0500-000000000000}">
   <dimension ref="A1:I2"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="A2" sqref="A2:XFD2"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="A2" sqref="A2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="15"/>

</xml_diff>

<commit_message>
Added the slido comments to the respective sessions
</commit_message>
<xml_diff>
--- a/2019/slido/Questions-SCAM 2019.xlsx
+++ b/2019/slido/Questions-SCAM 2019.xlsx
@@ -1,11 +1,10 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="5" rupBuild="21425"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
+  <fileVersion appName="xl" lastEdited="6" lowestEdited="5" rupBuild="14420"/>
   <workbookPr filterPrivacy="1"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1DE04CF5-8BD4-4C8D-A2D3-5579D748432B}" xr6:coauthVersionLast="43" xr6:coauthVersionMax="43" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" firstSheet="1" activeTab="4" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" activeTab="5"/>
   </bookViews>
   <sheets>
     <sheet name="Program Analysis" sheetId="2" r:id="rId1"/>
@@ -388,7 +387,7 @@
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
   <fonts count="3">
     <font>
       <sz val="11"/>
@@ -773,7 +772,7 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:I20"/>
   <sheetViews>
     <sheetView workbookViewId="0">
@@ -1380,7 +1379,7 @@
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0200-000000000000}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:I14"/>
   <sheetViews>
     <sheetView workbookViewId="0">
@@ -1813,7 +1812,7 @@
 </file>
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0300-000000000000}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:I7"/>
   <sheetViews>
     <sheetView workbookViewId="0">
@@ -2043,7 +2042,7 @@
 </file>
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0400-000000000000}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:I1"/>
   <sheetViews>
     <sheetView workbookViewId="0">
@@ -2099,10 +2098,10 @@
 </file>
 
 <file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0500-000000000000}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:I2"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="A2" sqref="A2"/>
     </sheetView>
   </sheetViews>
@@ -2184,10 +2183,10 @@
 </file>
 
 <file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0600-000000000000}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:H3"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
+    <sheetView tabSelected="1" workbookViewId="0">
       <selection activeCell="A3" sqref="A3"/>
     </sheetView>
   </sheetViews>

</xml_diff>